<commit_message>
update paket menu fixed
</commit_message>
<xml_diff>
--- a/public/files/inetwork_paket_import_template_fix.xlsx
+++ b/public/files/inetwork_paket_import_template_fix.xlsx
@@ -1021,13 +1021,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="1" width="3.425" customWidth="true"/>
     <col min="2" max="2" width="7" customWidth="true"/>
@@ -1087,17 +1087,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>100000</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>